<commit_message>
April 5 update 2
</commit_message>
<xml_diff>
--- a/Jupyter/simulationID/cim_0326_1234/data/script_ssi.xlsx
+++ b/Jupyter/simulationID/cim_0326_1234/data/script_ssi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shai/Google Drive/BatYam NY DRIVE/Simulations/March 14 GitHUB/BatYamNY/Jupyter/simulationID/cim_0326_1234/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60A565E-E352-5749-AE0A-7014BC9A9DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BFFB8D-E036-C94E-9A2A-AB5F2954DE88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-2680" windowWidth="33600" windowHeight="20540" xr2:uid="{A86D1036-0752-124D-A288-1321B8986789}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="97">
   <si>
     <t>index</t>
   </si>
@@ -318,6 +318,12 @@
   </si>
   <si>
     <t>34,31</t>
+  </si>
+  <si>
+    <t>NewNonRentCost</t>
+  </si>
+  <si>
+    <t>NewRentCost</t>
   </si>
 </sst>
 </file>
@@ -819,13 +825,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807C292D-0617-114F-905A-ECB223F31F24}">
-  <dimension ref="A1:AH27"/>
+  <dimension ref="A1:AJ27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC32" sqref="AC32"/>
+      <selection pane="bottomRight" activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,7 +855,7 @@
     <col min="32" max="32" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -952,8 +958,14 @@
       <c r="AH1" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="AI1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1064,8 +1076,16 @@
         <f t="shared" ref="AH2:AH15" si="1">J2*AB2</f>
         <v>543.58000000000004</v>
       </c>
+      <c r="AI2">
+        <f>AH2+AG2</f>
+        <v>723.58</v>
+      </c>
+      <c r="AJ2">
+        <f>AH2+AG2+AE2</f>
+        <v>7723.5800000000008</v>
+      </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1176,8 +1196,16 @@
         <f t="shared" si="1"/>
         <v>733.83300000000008</v>
       </c>
+      <c r="AI3">
+        <f t="shared" ref="AI3:AI25" si="6">AH3+AG3</f>
+        <v>913.83300000000008</v>
+      </c>
+      <c r="AJ3">
+        <f t="shared" ref="AJ3:AJ25" si="7">AH3+AG3+AE3</f>
+        <v>11191.833000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1288,8 +1316,16 @@
         <f t="shared" si="1"/>
         <v>576.19479999999999</v>
       </c>
+      <c r="AI4">
+        <f t="shared" si="6"/>
+        <v>756.19479999999999</v>
+      </c>
+      <c r="AJ4">
+        <f t="shared" si="7"/>
+        <v>8748.3948</v>
+      </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1323,7 +1359,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K5" s="7">
-        <f t="shared" ref="K5:K22" si="6">INT(J5*F5)</f>
+        <f t="shared" ref="K5:K22" si="8">INT(J5*F5)</f>
         <v>407</v>
       </c>
       <c r="L5">
@@ -1399,8 +1435,16 @@
         <f t="shared" si="1"/>
         <v>543.58000000000004</v>
       </c>
+      <c r="AI5">
+        <f t="shared" si="6"/>
+        <v>723.58</v>
+      </c>
+      <c r="AJ5">
+        <f t="shared" si="7"/>
+        <v>7503.5800000000008</v>
+      </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1434,7 +1478,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K6" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>434</v>
       </c>
       <c r="L6">
@@ -1511,8 +1555,16 @@
         <f t="shared" si="1"/>
         <v>500.09360000000004</v>
       </c>
+      <c r="AI6">
+        <f t="shared" si="6"/>
+        <v>680.09360000000004</v>
+      </c>
+      <c r="AJ6">
+        <f t="shared" si="7"/>
+        <v>6932.0936000000002</v>
+      </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1545,7 +1597,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K7" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>510</v>
       </c>
       <c r="L7">
@@ -1553,11 +1605,11 @@
         <v>1795556.6666666667</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M7:M22" si="7">H7*F7+I7+K7</f>
+        <f t="shared" ref="M7:M22" si="9">H7*F7+I7+K7</f>
         <v>5310</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N22" si="8">K7+I7</f>
+        <f t="shared" ref="N7:N22" si="10">K7+I7</f>
         <v>610</v>
       </c>
       <c r="O7">
@@ -1622,8 +1674,16 @@
         <f t="shared" si="1"/>
         <v>646.86020000000008</v>
       </c>
+      <c r="AI7">
+        <f t="shared" si="6"/>
+        <v>966.86020000000008</v>
+      </c>
+      <c r="AJ7">
+        <f t="shared" si="7"/>
+        <v>8426.8601999999992</v>
+      </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1658,7 +1718,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K8" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>407</v>
       </c>
       <c r="L8">
@@ -1666,11 +1726,11 @@
         <v>1491812.5000000002</v>
       </c>
       <c r="M8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5832</v>
       </c>
       <c r="N8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>507</v>
       </c>
       <c r="O8">
@@ -1735,8 +1795,16 @@
         <f t="shared" si="1"/>
         <v>472.91460000000006</v>
       </c>
+      <c r="AI8">
+        <f t="shared" si="6"/>
+        <v>652.91460000000006</v>
+      </c>
+      <c r="AJ8">
+        <f t="shared" si="7"/>
+        <v>8245.3145999999997</v>
+      </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1769,7 +1837,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K9" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>462</v>
       </c>
       <c r="L9">
@@ -1777,11 +1845,11 @@
         <v>1560370.3299999998</v>
       </c>
       <c r="M9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5832</v>
       </c>
       <c r="N9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>562</v>
       </c>
       <c r="O9">
@@ -1846,8 +1914,16 @@
         <f t="shared" si="1"/>
         <v>527.27260000000001</v>
       </c>
+      <c r="AI9">
+        <f t="shared" si="6"/>
+        <v>707.27260000000001</v>
+      </c>
+      <c r="AJ9">
+        <f t="shared" si="7"/>
+        <v>8104.0725999999995</v>
+      </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1881,7 +1957,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K10" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>353</v>
       </c>
       <c r="L10">
@@ -1889,11 +1965,11 @@
         <v>1191384.4041666666</v>
       </c>
       <c r="M10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4808</v>
       </c>
       <c r="N10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>453</v>
       </c>
       <c r="O10">
@@ -1958,8 +2034,16 @@
         <f t="shared" si="1"/>
         <v>652.29600000000005</v>
       </c>
+      <c r="AI10">
+        <f t="shared" si="6"/>
+        <v>972.29600000000005</v>
+      </c>
+      <c r="AJ10">
+        <f t="shared" si="7"/>
+        <v>10940.296</v>
+      </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1992,7 +2076,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K11" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>462</v>
       </c>
       <c r="L11">
@@ -2000,11 +2084,11 @@
         <v>1687985.5049999999</v>
       </c>
       <c r="M11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6087</v>
       </c>
       <c r="N11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>562</v>
       </c>
       <c r="O11">
@@ -2069,8 +2153,16 @@
         <f t="shared" si="1"/>
         <v>543.58000000000004</v>
       </c>
+      <c r="AI11">
+        <f t="shared" si="6"/>
+        <v>723.58</v>
+      </c>
+      <c r="AJ11">
+        <f t="shared" si="7"/>
+        <v>8053.5800000000008</v>
+      </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2104,7 +2196,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K12" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>423</v>
       </c>
       <c r="L12">
@@ -2112,11 +2204,11 @@
         <v>1612750.5420000001</v>
       </c>
       <c r="M12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5359</v>
       </c>
       <c r="N12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>523</v>
       </c>
       <c r="O12" s="8">
@@ -2181,8 +2273,16 @@
         <f t="shared" si="1"/>
         <v>489.22200000000004</v>
       </c>
+      <c r="AI12">
+        <f t="shared" si="6"/>
+        <v>669.22199999999998</v>
+      </c>
+      <c r="AJ12">
+        <f t="shared" si="7"/>
+        <v>6987.2220000000007</v>
+      </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2216,7 +2316,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K13" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>451</v>
       </c>
       <c r="L13">
@@ -2224,11 +2324,11 @@
         <v>1587799.8908333334</v>
       </c>
       <c r="M13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4950</v>
       </c>
       <c r="N13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>551</v>
       </c>
       <c r="O13" s="8">
@@ -2293,8 +2393,16 @@
         <f t="shared" si="1"/>
         <v>516.40100000000007</v>
       </c>
+      <c r="AI13">
+        <f t="shared" si="6"/>
+        <v>696.40100000000007</v>
+      </c>
+      <c r="AJ13">
+        <f t="shared" si="7"/>
+        <v>6414.9010000000007</v>
+      </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2328,7 +2436,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>402</v>
       </c>
       <c r="L14">
@@ -2336,11 +2444,11 @@
         <v>1438701.0933333335</v>
       </c>
       <c r="M14" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5312</v>
       </c>
       <c r="N14" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>502</v>
       </c>
       <c r="O14" s="8">
@@ -2405,8 +2513,16 @@
         <f t="shared" si="1"/>
         <v>467.47880000000004</v>
       </c>
+      <c r="AI14">
+        <f t="shared" si="6"/>
+        <v>647.47880000000009</v>
+      </c>
+      <c r="AJ14">
+        <f t="shared" si="7"/>
+        <v>6976.4788000000008</v>
+      </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2439,7 +2555,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K15" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>440</v>
       </c>
       <c r="L15">
@@ -2447,11 +2563,11 @@
         <v>1547950.743</v>
       </c>
       <c r="M15" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5805</v>
       </c>
       <c r="N15" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>540</v>
       </c>
       <c r="O15">
@@ -2516,8 +2632,16 @@
         <f t="shared" si="1"/>
         <v>505.52940000000001</v>
       </c>
+      <c r="AI15">
+        <f t="shared" si="6"/>
+        <v>685.52940000000001</v>
+      </c>
+      <c r="AJ15">
+        <f t="shared" si="7"/>
+        <v>7515.0294000000013</v>
+      </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2550,7 +2674,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K16" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>434</v>
       </c>
       <c r="L16">
@@ -2558,11 +2682,11 @@
         <v>1885658.8800000001</v>
       </c>
       <c r="M16" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5734</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>534</v>
       </c>
       <c r="O16" s="8">
@@ -2627,8 +2751,16 @@
         <f>J16*AB16</f>
         <v>652.29600000000005</v>
       </c>
+      <c r="AI16">
+        <f t="shared" si="6"/>
+        <v>1102.296</v>
+      </c>
+      <c r="AJ16">
+        <f t="shared" si="7"/>
+        <v>66352.296000000002</v>
+      </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2662,7 +2794,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K17" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>353</v>
       </c>
       <c r="L17">
@@ -2670,11 +2802,11 @@
         <v>1289166.6666666667</v>
       </c>
       <c r="M17" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4548</v>
       </c>
       <c r="N17" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>453</v>
       </c>
       <c r="O17" s="8">
@@ -2739,8 +2871,16 @@
         <f>J17*AB17</f>
         <v>652.29600000000005</v>
       </c>
+      <c r="AI17">
+        <f t="shared" si="6"/>
+        <v>1102.296</v>
+      </c>
+      <c r="AJ17">
+        <f t="shared" si="7"/>
+        <v>66352.296000000002</v>
+      </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2774,7 +2914,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>462</v>
       </c>
       <c r="L18">
@@ -2782,11 +2922,11 @@
         <v>1801643.0772727272</v>
       </c>
       <c r="M18" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6087</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>562</v>
       </c>
       <c r="O18" s="8">
@@ -2851,8 +2991,16 @@
         <f>J18*AB18</f>
         <v>527.27260000000001</v>
       </c>
+      <c r="AI18">
+        <f t="shared" si="6"/>
+        <v>727.27260000000001</v>
+      </c>
+      <c r="AJ18">
+        <f t="shared" si="7"/>
+        <v>7862.7726000000002</v>
+      </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2885,7 +3033,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K19" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>391</v>
       </c>
       <c r="L19" s="6">
@@ -2893,11 +3041,11 @@
         <v>1536192</v>
       </c>
       <c r="M19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4955</v>
       </c>
       <c r="N19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>491</v>
       </c>
       <c r="O19" s="8">
@@ -2959,11 +3107,19 @@
         <v>450</v>
       </c>
       <c r="AH19">
-        <f t="shared" ref="AH19:AH25" si="9">J19*AB19</f>
+        <f t="shared" ref="AH19:AH25" si="11">J19*AB19</f>
         <v>652.29600000000005</v>
       </c>
+      <c r="AI19">
+        <f t="shared" si="6"/>
+        <v>1102.296</v>
+      </c>
+      <c r="AJ19">
+        <f t="shared" si="7"/>
+        <v>71752.296000000002</v>
+      </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2996,7 +3152,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K20" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>445</v>
       </c>
       <c r="L20" s="6">
@@ -3004,11 +3160,11 @@
         <v>1906254</v>
       </c>
       <c r="M20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5629</v>
       </c>
       <c r="N20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>545</v>
       </c>
       <c r="O20" s="8">
@@ -3069,11 +3225,19 @@
         <v>450</v>
       </c>
       <c r="AH20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>652.29600000000005</v>
       </c>
+      <c r="AI20">
+        <f t="shared" si="6"/>
+        <v>1102.296</v>
+      </c>
+      <c r="AJ20">
+        <f t="shared" si="7"/>
+        <v>71752.296000000002</v>
+      </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3106,7 +3270,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K21" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>543</v>
       </c>
       <c r="L21" s="6">
@@ -3114,11 +3278,11 @@
         <v>2087800</v>
       </c>
       <c r="M21" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7043</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>643</v>
       </c>
       <c r="O21">
@@ -3180,11 +3344,19 @@
         <v>320</v>
       </c>
       <c r="AH21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>543.58000000000004</v>
       </c>
+      <c r="AI21">
+        <f t="shared" si="6"/>
+        <v>863.58</v>
+      </c>
+      <c r="AJ21">
+        <f t="shared" si="7"/>
+        <v>8223.5800000000017</v>
+      </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3218,7 +3390,7 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K22" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>478</v>
       </c>
       <c r="L22" s="6">
@@ -3226,11 +3398,11 @@
         <v>1746800</v>
       </c>
       <c r="M22" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5858</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>578</v>
       </c>
       <c r="O22">
@@ -3292,11 +3464,19 @@
         <v>320</v>
       </c>
       <c r="AH22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>652.29600000000005</v>
       </c>
+      <c r="AI22">
+        <f t="shared" si="6"/>
+        <v>972.29600000000005</v>
+      </c>
+      <c r="AJ22">
+        <f t="shared" si="7"/>
+        <v>9212.2960000000003</v>
+      </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3329,19 +3509,19 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K23" s="10">
-        <f t="shared" ref="K23:K25" si="10">INT(J23*F23)</f>
+        <f t="shared" ref="K23:K25" si="12">INT(J23*F23)</f>
         <v>472</v>
       </c>
       <c r="L23" s="6">
-        <f t="shared" ref="L23:L25" si="11">G23*F23</f>
+        <f t="shared" ref="L23:L25" si="13">G23*F23</f>
         <v>1748119.449</v>
       </c>
       <c r="M23" s="10">
-        <f t="shared" ref="M23:M25" si="12">H23*F23+I23+K23</f>
+        <f t="shared" ref="M23:M25" si="14">H23*F23+I23+K23</f>
         <v>6140</v>
       </c>
       <c r="N23" s="10">
-        <f t="shared" ref="N23:N25" si="13">K23+I23</f>
+        <f t="shared" ref="N23:N25" si="15">K23+I23</f>
         <v>572</v>
       </c>
       <c r="O23">
@@ -3403,11 +3583,19 @@
         <v>180</v>
       </c>
       <c r="AH23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>538.14420000000007</v>
       </c>
+      <c r="AI23">
+        <f t="shared" si="6"/>
+        <v>718.14420000000007</v>
+      </c>
+      <c r="AJ23">
+        <f t="shared" si="7"/>
+        <v>7867.7442000000001</v>
+      </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3441,19 +3629,19 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K24" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>358</v>
       </c>
       <c r="L24" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1202960</v>
       </c>
       <c r="M24" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4616</v>
       </c>
       <c r="N24" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>458</v>
       </c>
       <c r="O24">
@@ -3515,11 +3703,19 @@
         <v>180</v>
       </c>
       <c r="AH24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>423.99240000000003</v>
       </c>
+      <c r="AI24">
+        <f t="shared" si="6"/>
+        <v>603.99240000000009</v>
+      </c>
+      <c r="AJ24">
+        <f t="shared" si="7"/>
+        <v>6189.3924000000006</v>
+      </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3553,19 +3749,19 @@
         <v>5.4358000000000004</v>
       </c>
       <c r="K25" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>418</v>
       </c>
       <c r="L25" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1364504.1666666667</v>
       </c>
       <c r="M25" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4907</v>
       </c>
       <c r="N25" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>518</v>
       </c>
       <c r="O25">
@@ -3627,11 +3823,19 @@
         <v>180</v>
       </c>
       <c r="AH25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>483.78620000000001</v>
       </c>
+      <c r="AI25">
+        <f t="shared" si="6"/>
+        <v>663.78620000000001</v>
+      </c>
+      <c r="AJ25">
+        <f t="shared" si="7"/>
+        <v>6424.0861999999997</v>
+      </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
     </row>
   </sheetData>

</xml_diff>